<commit_message>
modul 2 hampir selesai
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\eLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA2DCDE5-F3A8-44C3-BD50-9653668D3B83}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{52E8AB2B-8736-4D6A-9FE8-DD09DC286432}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{268EED0B-7FD1-4F01-9C2D-DEE4B3EFCE48}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="154">
   <si>
     <t>jessica</t>
   </si>
@@ -97,6 +97,396 @@
   </si>
   <si>
     <t>yamato.com</t>
+  </si>
+  <si>
+    <t>jl gabumon</t>
+  </si>
+  <si>
+    <t>gio</t>
+  </si>
+  <si>
+    <t>gio.com</t>
+  </si>
+  <si>
+    <t>jl raben</t>
+  </si>
+  <si>
+    <t>vivi</t>
+  </si>
+  <si>
+    <t>vivi.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jl raben 1 </t>
+  </si>
+  <si>
+    <t>ogi</t>
+  </si>
+  <si>
+    <t>ogi.com</t>
+  </si>
+  <si>
+    <t>jl rabon</t>
+  </si>
+  <si>
+    <t>ibu</t>
+  </si>
+  <si>
+    <t>ibu.com</t>
+  </si>
+  <si>
+    <t>jl ibu</t>
+  </si>
+  <si>
+    <t>ayah</t>
+  </si>
+  <si>
+    <t>ayah.com</t>
+  </si>
+  <si>
+    <t>jl ayah</t>
+  </si>
+  <si>
+    <t>kakak</t>
+  </si>
+  <si>
+    <t>jl kakak</t>
+  </si>
+  <si>
+    <t>kakak.com</t>
+  </si>
+  <si>
+    <t>adik</t>
+  </si>
+  <si>
+    <t>adik.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jl adik </t>
+  </si>
+  <si>
+    <t>agumon</t>
+  </si>
+  <si>
+    <t>agumon.com</t>
+  </si>
+  <si>
+    <t>jl agumon</t>
+  </si>
+  <si>
+    <t>biyomon</t>
+  </si>
+  <si>
+    <t>biyomon.com</t>
+  </si>
+  <si>
+    <t>jl biyomon</t>
+  </si>
+  <si>
+    <t>tentomon</t>
+  </si>
+  <si>
+    <t>tentomon.com</t>
+  </si>
+  <si>
+    <t>jl tentomon</t>
+  </si>
+  <si>
+    <t>patamon</t>
+  </si>
+  <si>
+    <t>patamon.com</t>
+  </si>
+  <si>
+    <t>jl patamon</t>
+  </si>
+  <si>
+    <t>gatomon</t>
+  </si>
+  <si>
+    <t>gatomon.com</t>
+  </si>
+  <si>
+    <t>jl gatomon</t>
+  </si>
+  <si>
+    <t>vmon</t>
+  </si>
+  <si>
+    <t>vmon.com</t>
+  </si>
+  <si>
+    <t>jl vmon</t>
+  </si>
+  <si>
+    <t>hawkmon</t>
+  </si>
+  <si>
+    <t>hawkmon.com</t>
+  </si>
+  <si>
+    <t>jl hawkmon</t>
+  </si>
+  <si>
+    <t>pikachu</t>
+  </si>
+  <si>
+    <t>pikachu.com</t>
+  </si>
+  <si>
+    <t>jl pikachu</t>
+  </si>
+  <si>
+    <t>guilmon</t>
+  </si>
+  <si>
+    <t>guilmon.com</t>
+  </si>
+  <si>
+    <t>jl guilmon</t>
+  </si>
+  <si>
+    <t>terriermon</t>
+  </si>
+  <si>
+    <t>terriermon.com</t>
+  </si>
+  <si>
+    <t>jl terriermon</t>
+  </si>
+  <si>
+    <t>renamon</t>
+  </si>
+  <si>
+    <t>renamon.com</t>
+  </si>
+  <si>
+    <t>jl renamon</t>
+  </si>
+  <si>
+    <t>agnimon</t>
+  </si>
+  <si>
+    <t>agnimon.com</t>
+  </si>
+  <si>
+    <t>jl agnimon</t>
+  </si>
+  <si>
+    <t>lobomon</t>
+  </si>
+  <si>
+    <t>lobomon.com</t>
+  </si>
+  <si>
+    <t>jl lobomon</t>
+  </si>
+  <si>
+    <t>chakmon</t>
+  </si>
+  <si>
+    <t>chakmon.com</t>
+  </si>
+  <si>
+    <t>jl chakmon</t>
+  </si>
+  <si>
+    <t>goku</t>
+  </si>
+  <si>
+    <t>goku.com</t>
+  </si>
+  <si>
+    <t>jl kurakura</t>
+  </si>
+  <si>
+    <t>bejita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bejita </t>
+  </si>
+  <si>
+    <t>bejita.com</t>
+  </si>
+  <si>
+    <t>jl bejita</t>
+  </si>
+  <si>
+    <t>piccolo</t>
+  </si>
+  <si>
+    <t>piccolo.com</t>
+  </si>
+  <si>
+    <t>picollo</t>
+  </si>
+  <si>
+    <t>jl piccolo</t>
+  </si>
+  <si>
+    <t>krillin</t>
+  </si>
+  <si>
+    <t>krillin.com</t>
+  </si>
+  <si>
+    <t>jl krillin</t>
+  </si>
+  <si>
+    <t>yamcha</t>
+  </si>
+  <si>
+    <t>yamcha.com</t>
+  </si>
+  <si>
+    <t>jl yamcha</t>
+  </si>
+  <si>
+    <t>tenshinhan</t>
+  </si>
+  <si>
+    <t>tenshinhan.com</t>
+  </si>
+  <si>
+    <t>jl tenshinhan</t>
+  </si>
+  <si>
+    <t>dotcom</t>
+  </si>
+  <si>
+    <t>dotcom.com</t>
+  </si>
+  <si>
+    <t>jl dotcom</t>
+  </si>
+  <si>
+    <t>fathia</t>
+  </si>
+  <si>
+    <t>fathia.com</t>
+  </si>
+  <si>
+    <t>jl fathia</t>
+  </si>
+  <si>
+    <t>tatjana</t>
+  </si>
+  <si>
+    <t>tatjana.com</t>
+  </si>
+  <si>
+    <t>jl tatjana</t>
+  </si>
+  <si>
+    <t>rehbo</t>
+  </si>
+  <si>
+    <t>rehbo.com</t>
+  </si>
+  <si>
+    <t>jl rehbo</t>
+  </si>
+  <si>
+    <t>anya</t>
+  </si>
+  <si>
+    <t>anya.com</t>
+  </si>
+  <si>
+    <t>jl anya</t>
+  </si>
+  <si>
+    <t>tasya</t>
+  </si>
+  <si>
+    <t>tasya.com</t>
+  </si>
+  <si>
+    <t>jl tasya</t>
+  </si>
+  <si>
+    <t>gunawan</t>
+  </si>
+  <si>
+    <t>gunawan.com</t>
+  </si>
+  <si>
+    <t>jl gunawan</t>
+  </si>
+  <si>
+    <t>obiwan</t>
+  </si>
+  <si>
+    <t>obiwan.com</t>
+  </si>
+  <si>
+    <t>jl obiwan</t>
+  </si>
+  <si>
+    <t>anain</t>
+  </si>
+  <si>
+    <t>anakin</t>
+  </si>
+  <si>
+    <t>anakin.com</t>
+  </si>
+  <si>
+    <t>jl anakin</t>
+  </si>
+  <si>
+    <t>yoda</t>
+  </si>
+  <si>
+    <t>yoda.com</t>
+  </si>
+  <si>
+    <t>jl yoda</t>
+  </si>
+  <si>
+    <t>jarjar</t>
+  </si>
+  <si>
+    <t>jarjar.com</t>
+  </si>
+  <si>
+    <t>jl jarjar</t>
+  </si>
+  <si>
+    <t>hansolos</t>
+  </si>
+  <si>
+    <t>hansolo</t>
+  </si>
+  <si>
+    <t>hansolo.com</t>
+  </si>
+  <si>
+    <t>jl hansolo</t>
+  </si>
+  <si>
+    <t>vader</t>
+  </si>
+  <si>
+    <t>vader.com</t>
+  </si>
+  <si>
+    <t>jl vader</t>
+  </si>
+  <si>
+    <t>leia</t>
+  </si>
+  <si>
+    <t>leia.com</t>
+  </si>
+  <si>
+    <t>jl leia</t>
+  </si>
+  <si>
+    <t>finn</t>
+  </si>
+  <si>
+    <t>jl finn</t>
   </si>
 </sst>
 </file>
@@ -448,13 +838,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C222129B-E0E1-413A-867E-3E9B5954BF85}">
-  <dimension ref="B1:H16"/>
+  <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -492,6 +889,199 @@
       <c r="E2" t="s">
         <v>22</v>
       </c>
+      <c r="F2">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>9823</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>2093</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <v>999</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7">
+        <v>1230</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>2304</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9">
+        <v>324</v>
+      </c>
+      <c r="G9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10">
+        <v>992</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -628,6 +1218,788 @@
         <v>18</v>
       </c>
       <c r="H16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17">
+        <v>123</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18">
+        <v>234</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19">
+        <v>8878</v>
+      </c>
+      <c r="G19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20">
+        <v>77673</v>
+      </c>
+      <c r="G20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21">
+        <v>998</v>
+      </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22">
+        <v>676</v>
+      </c>
+      <c r="G22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23">
+        <v>123</v>
+      </c>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24">
+        <v>123</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25">
+        <v>600</v>
+      </c>
+      <c r="G25" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26">
+        <v>234</v>
+      </c>
+      <c r="G26" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27">
+        <v>5342</v>
+      </c>
+      <c r="G27" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28">
+        <v>7238</v>
+      </c>
+      <c r="G28" t="s">
+        <v>84</v>
+      </c>
+      <c r="H28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29">
+        <v>900</v>
+      </c>
+      <c r="G29" t="s">
+        <v>87</v>
+      </c>
+      <c r="H29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30">
+        <v>81023</v>
+      </c>
+      <c r="G30" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31">
+        <v>234</v>
+      </c>
+      <c r="G31" t="s">
+        <v>94</v>
+      </c>
+      <c r="H31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32">
+        <v>123</v>
+      </c>
+      <c r="G32" t="s">
+        <v>98</v>
+      </c>
+      <c r="H32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33">
+        <v>3729</v>
+      </c>
+      <c r="G33" t="s">
+        <v>101</v>
+      </c>
+      <c r="H33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34">
+        <v>324</v>
+      </c>
+      <c r="G34" t="s">
+        <v>104</v>
+      </c>
+      <c r="H34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35">
+        <v>990</v>
+      </c>
+      <c r="G35" t="s">
+        <v>107</v>
+      </c>
+      <c r="H35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" t="s">
+        <v>108</v>
+      </c>
+      <c r="F36">
+        <v>911</v>
+      </c>
+      <c r="G36" t="s">
+        <v>110</v>
+      </c>
+      <c r="H36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37">
+        <v>888</v>
+      </c>
+      <c r="G37" t="s">
+        <v>113</v>
+      </c>
+      <c r="H37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" t="s">
+        <v>114</v>
+      </c>
+      <c r="F38">
+        <v>999</v>
+      </c>
+      <c r="G38" t="s">
+        <v>116</v>
+      </c>
+      <c r="H38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F39">
+        <v>787</v>
+      </c>
+      <c r="G39" t="s">
+        <v>119</v>
+      </c>
+      <c r="H39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" t="s">
+        <v>121</v>
+      </c>
+      <c r="E40" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40">
+        <v>678</v>
+      </c>
+      <c r="G40" t="s">
+        <v>122</v>
+      </c>
+      <c r="H40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" t="s">
+        <v>123</v>
+      </c>
+      <c r="F41">
+        <v>567</v>
+      </c>
+      <c r="G41" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" t="s">
+        <v>126</v>
+      </c>
+      <c r="F42">
+        <v>456</v>
+      </c>
+      <c r="G42" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" t="s">
+        <v>130</v>
+      </c>
+      <c r="E43" t="s">
+        <v>129</v>
+      </c>
+      <c r="F43">
+        <v>222</v>
+      </c>
+      <c r="G43" t="s">
+        <v>131</v>
+      </c>
+      <c r="H43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" t="s">
+        <v>133</v>
+      </c>
+      <c r="F44">
+        <v>66</v>
+      </c>
+      <c r="G44" t="s">
+        <v>135</v>
+      </c>
+      <c r="H44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45">
+        <v>3333</v>
+      </c>
+      <c r="G45" t="s">
+        <v>138</v>
+      </c>
+      <c r="H45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" t="s">
+        <v>140</v>
+      </c>
+      <c r="E46" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46">
+        <v>4769</v>
+      </c>
+      <c r="G46" t="s">
+        <v>141</v>
+      </c>
+      <c r="H46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" t="s">
+        <v>143</v>
+      </c>
+      <c r="F47">
+        <v>1212</v>
+      </c>
+      <c r="G47" t="s">
+        <v>145</v>
+      </c>
+      <c r="H47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" t="s">
+        <v>147</v>
+      </c>
+      <c r="E48" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48">
+        <v>666</v>
+      </c>
+      <c r="G48" t="s">
+        <v>148</v>
+      </c>
+      <c r="H48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" t="s">
+        <v>150</v>
+      </c>
+      <c r="E49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F49">
+        <v>303</v>
+      </c>
+      <c r="G49" t="s">
+        <v>151</v>
+      </c>
+      <c r="H49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>152</v>
+      </c>
+      <c r="F50">
+        <v>218</v>
+      </c>
+      <c r="G50" t="s">
+        <v>153</v>
+      </c>
+      <c r="H50" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>